<commit_message>
added initials and updated template
</commit_message>
<xml_diff>
--- a/src/assets/template.xlsx
+++ b/src/assets/template.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Abubakar.NOTEBOOK\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{750CC95B-5AE0-400A-B4D9-3FC090E6369E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A364DF91-E11B-4D8D-A0A6-803F8282D22A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{4E254CAC-24CF-42AA-A9D0-CDC25810A912}"/>
+    <workbookView xWindow="2730" yWindow="2730" windowWidth="15375" windowHeight="8325" activeTab="1" xr2:uid="{4E254CAC-24CF-42AA-A9D0-CDC25810A912}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Initials" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="35">
   <si>
     <t>English</t>
   </si>
@@ -99,6 +100,48 @@
   </si>
   <si>
     <t>Total Marks</t>
+  </si>
+  <si>
+    <t>Subject</t>
+  </si>
+  <si>
+    <t>Initial</t>
+  </si>
+  <si>
+    <t>ENGLISH</t>
+  </si>
+  <si>
+    <t>KISWAHILI</t>
+  </si>
+  <si>
+    <t>MATHEMATICS</t>
+  </si>
+  <si>
+    <t>BIOLOGY</t>
+  </si>
+  <si>
+    <t>CHEMISTRY</t>
+  </si>
+  <si>
+    <t>PHYSICS</t>
+  </si>
+  <si>
+    <t xml:space="preserve">HISTORY &amp; GOVT </t>
+  </si>
+  <si>
+    <t>GEOGRAPHY</t>
+  </si>
+  <si>
+    <t>AGRICULTURE</t>
+  </si>
+  <si>
+    <t>COMPUTER STUDIES</t>
+  </si>
+  <si>
+    <t>BUSINESS STUDIES</t>
+  </si>
+  <si>
+    <t>ARABIC</t>
   </si>
 </sst>
 </file>
@@ -419,10 +462,10 @@
     <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="15" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -443,6 +486,17 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{76593677-2054-4020-8AA5-51E19E60CD0A}" name="Table1" displayName="Table1" ref="A1:B14" totalsRowShown="0">
+  <autoFilter ref="A1:B14" xr:uid="{76593677-2054-4020-8AA5-51E19E60CD0A}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9EFE548C-8944-4F6E-A4D3-EE1DB28A5C01}" name="Subject"/>
+    <tableColumn id="2" xr3:uid="{B3F5FCC9-F52A-4ACD-B9CB-2C0C32313601}" name="Initial"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -744,8 +798,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{92599EC8-95C9-4E35-91DC-F76F09EDAEED}">
   <dimension ref="A1:AD70"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -765,56 +819,56 @@
       <c r="D1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="E1" s="17"/>
+      <c r="E1" s="18"/>
       <c r="F1" s="15" t="s">
         <v>11</v>
       </c>
-      <c r="G1" s="17"/>
+      <c r="G1" s="18"/>
       <c r="H1" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="I1" s="17"/>
+      <c r="I1" s="18"/>
       <c r="J1" s="15" t="s">
         <v>3</v>
       </c>
-      <c r="K1" s="17"/>
+      <c r="K1" s="18"/>
       <c r="L1" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="M1" s="17"/>
+      <c r="M1" s="18"/>
       <c r="N1" s="15" t="s">
         <v>1</v>
       </c>
-      <c r="O1" s="17"/>
+      <c r="O1" s="18"/>
       <c r="P1" s="15" t="s">
         <v>12</v>
       </c>
-      <c r="Q1" s="17"/>
+      <c r="Q1" s="18"/>
       <c r="R1" s="15" t="s">
         <v>19</v>
       </c>
-      <c r="S1" s="17"/>
+      <c r="S1" s="18"/>
       <c r="T1" s="15" t="s">
         <v>13</v>
       </c>
-      <c r="U1" s="17"/>
+      <c r="U1" s="18"/>
       <c r="V1" s="15" t="s">
         <v>14</v>
       </c>
-      <c r="W1" s="17"/>
+      <c r="W1" s="18"/>
       <c r="X1" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="Y1" s="17"/>
+      <c r="Y1" s="18"/>
       <c r="Z1" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="AA1" s="17"/>
+      <c r="AA1" s="18"/>
       <c r="AB1" s="15" t="s">
         <v>17</v>
       </c>
       <c r="AC1" s="16"/>
-      <c r="AD1" s="18" t="s">
+      <c r="AD1" s="17" t="s">
         <v>20</v>
       </c>
     </row>
@@ -906,7 +960,7 @@
       <c r="AC2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="AD2" s="18"/>
+      <c r="AD2" s="17"/>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3" s="4"/>
@@ -974,7 +1028,7 @@
       <c r="AB4" s="6"/>
       <c r="AC4" s="6"/>
       <c r="AD4">
-        <f t="shared" ref="AD4:AD60" si="0">SUM(D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4,O4,P4,Q4,R4,S4,T4,U4,V4,W4,X4,Y4,Z4,AA4,AB4,AC4)</f>
+        <f t="shared" ref="AD4:AD11" si="0">SUM(D4,E4,F4,G4,H4,I4,J4,K4,L4,M4,N4,O4,P4,Q4,R4,S4,T4,U4,V4,W4,X4,Y4,Z4,AA4,AB4,AC4)</f>
         <v>0</v>
       </c>
     </row>
@@ -3316,4 +3370,99 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6BDBF9B4-5C88-4FE9-9B5A-C2D1B5C68FC5}">
+  <dimension ref="A1:B14"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="17.5703125" customWidth="1"/>
+    <col min="2" max="2" width="17.7109375" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
 </file>
</xml_diff>